<commit_message>
add code for global simulation climate data plots
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/korean-archaeologica-sites.xlsx
+++ b/analysis/data/raw_data/korean-archaeologica-sites.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7F5D4C-85BB-9145-9E2A-028CFB266EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="510" windowWidth="17895" windowHeight="7890"/>
+    <workbookView xWindow="5740" yWindow="920" windowWidth="21240" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="136">
   <si>
     <t>site_name</t>
   </si>
@@ -365,9 +371,6 @@
   </si>
   <si>
     <t>29,340±700</t>
-  </si>
-  <si>
-    <t>207-208</t>
   </si>
   <si>
     <t>127° 55′</t>
@@ -430,7 +433,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -504,6 +507,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -551,7 +557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,9 +590,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -619,6 +642,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,23 +834,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -862,7 +902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -886,7 +926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -910,7 +950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -936,7 +976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -962,7 +1002,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -986,7 +1026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1010,7 +1050,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1034,7 +1074,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1058,7 +1098,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1084,7 +1124,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1110,7 +1150,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>62</v>
       </c>
@@ -1134,7 +1174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -1158,7 +1198,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -1184,7 +1224,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>77</v>
       </c>
@@ -1208,7 +1248,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>82</v>
       </c>
@@ -1232,7 +1272,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>87</v>
       </c>
@@ -1256,7 +1296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -1280,7 +1320,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
@@ -1304,7 +1344,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
@@ -1330,7 +1370,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>108</v>
       </c>
@@ -1354,7 +1394,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
@@ -1378,7 +1418,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>115</v>
       </c>
@@ -1388,98 +1428,98 @@
       <c r="C24" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="1">
+        <v>207.5</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D25" s="1">
         <v>187</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G25" s="1">
         <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="D26" s="6">
         <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="G26" s="1">
         <v>5</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="D27" s="1">
         <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G27" s="1">
         <v>40</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the site name
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/korean-archaeologica-sites.xlsx
+++ b/analysis/data/raw_data/korean-archaeologica-sites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7F5D4C-85BB-9145-9E2A-028CFB266EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CD044A-9CA0-AB4C-BF26-97C89F7DB473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="920" windowWidth="21240" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21880" yWindow="2500" windowWidth="21240" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>site_name</t>
   </si>
@@ -64,9 +64,6 @@
     <t>호남문화재연구원 등 2008</t>
   </si>
   <si>
-    <t>Hahwagye-ri 3rd</t>
-  </si>
-  <si>
     <t>40,690±1,500</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>최복규 외 2004</t>
   </si>
   <si>
-    <t>Gihwa-ri Cave</t>
-  </si>
-  <si>
     <t>39,280±470</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>박영철 등 2007</t>
   </si>
   <si>
-    <t>Suyanggae location3 (redbrown layer)</t>
-  </si>
-  <si>
     <t>OSL</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t>이융조 외(한국선사문화연구원) 2013 3지구</t>
   </si>
   <si>
-    <t>Yongho-dong</t>
-  </si>
-  <si>
     <t>38,500±1,000</t>
   </si>
   <si>
@@ -127,9 +115,6 @@
     <t>한창균 2002</t>
   </si>
   <si>
-    <t>Galdun 4th Layer</t>
-  </si>
-  <si>
     <t>37,300±400</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>강원문화재연구소 2005</t>
   </si>
   <si>
-    <t>Cheon-ri</t>
-  </si>
-  <si>
     <t>36,000±4000</t>
   </si>
   <si>
@@ -172,24 +154,6 @@
     <t>경희대학교 중앙박물관 2013</t>
   </si>
   <si>
-    <t>Haga</t>
-  </si>
-  <si>
-    <t>34,900±400</t>
-  </si>
-  <si>
-    <t>127°13'12.6"</t>
-  </si>
-  <si>
-    <t>35°38'57.5"</t>
-  </si>
-  <si>
-    <t>이기길 한국고고학전국대회 32</t>
-  </si>
-  <si>
-    <t>Songam-ri 2nd</t>
-  </si>
-  <si>
     <t>33,190±160</t>
   </si>
   <si>
@@ -202,15 +166,6 @@
     <t>한국선사문화연구원 2012</t>
   </si>
   <si>
-    <t>Songam-ri 1st</t>
-  </si>
-  <si>
-    <t>32,300±160</t>
-  </si>
-  <si>
-    <t>Gawol-ri</t>
-  </si>
-  <si>
     <t>32,000±800</t>
   </si>
   <si>
@@ -223,9 +178,6 @@
     <t>국방문화재연구원 2010</t>
   </si>
   <si>
-    <t>Nosan-ri</t>
-  </si>
-  <si>
     <t>31,700±900</t>
   </si>
   <si>
@@ -238,9 +190,6 @@
     <t>이융조 2002</t>
   </si>
   <si>
-    <t>Hwadae-ri</t>
-  </si>
-  <si>
     <t>31,200±900</t>
   </si>
   <si>
@@ -253,24 +202,6 @@
     <t>최복규,유혜정 2005</t>
   </si>
   <si>
-    <t>Jeogok-ri</t>
-  </si>
-  <si>
-    <t>31,000±600</t>
-  </si>
-  <si>
-    <t>127° 02′</t>
-  </si>
-  <si>
-    <t>38° 02′</t>
-  </si>
-  <si>
-    <t>Vasilchuck et al. 2002</t>
-  </si>
-  <si>
-    <t>Sageun-ri</t>
-  </si>
-  <si>
     <t>30,800±300</t>
   </si>
   <si>
@@ -283,27 +214,6 @@
     <t>전북문화재연구원 2006</t>
   </si>
   <si>
-    <t>Seokjang-ri</t>
-  </si>
-  <si>
-    <t>β-ray</t>
-  </si>
-  <si>
-    <t>30,690±3,000</t>
-  </si>
-  <si>
-    <t>127°11'22.6"</t>
-  </si>
-  <si>
-    <t>36°26'51.3"</t>
-  </si>
-  <si>
-    <t>손보기 1993</t>
-  </si>
-  <si>
-    <t>Geumpa-ri</t>
-  </si>
-  <si>
     <t>30,800±100</t>
   </si>
   <si>
@@ -316,9 +226,6 @@
     <t>Bae et al. 2006</t>
   </si>
   <si>
-    <t>Ssangjung-ri</t>
-  </si>
-  <si>
     <t>30,220±150</t>
   </si>
   <si>
@@ -331,9 +238,6 @@
     <t>전라문화연구원 2012</t>
   </si>
   <si>
-    <t xml:space="preserve">Hopyeong-dong </t>
-  </si>
-  <si>
     <t>27,500±300</t>
   </si>
   <si>
@@ -346,9 +250,6 @@
     <t>경기문화재연구원 2010</t>
   </si>
   <si>
-    <t>Jeungsan-ri</t>
-  </si>
-  <si>
     <t>29,800±1,500</t>
   </si>
   <si>
@@ -361,15 +262,6 @@
     <t>호남문화재연구원 등 2011</t>
   </si>
   <si>
-    <t>Galdun 3th Layer</t>
-  </si>
-  <si>
-    <t>29,900±100</t>
-  </si>
-  <si>
-    <t>Jungjang-ri</t>
-  </si>
-  <si>
     <t>29,340±700</t>
   </si>
   <si>
@@ -428,13 +320,67 @@
   </si>
   <si>
     <t>중앙문화재연구원 2007</t>
+  </si>
+  <si>
+    <t>Hahwagyeri</t>
+  </si>
+  <si>
+    <t>Gihwari</t>
+  </si>
+  <si>
+    <t>Suyanggae</t>
+  </si>
+  <si>
+    <t>Yonghodong</t>
+  </si>
+  <si>
+    <t>Galdun</t>
+  </si>
+  <si>
+    <t>Cheonri</t>
+  </si>
+  <si>
+    <t>Songamri</t>
+  </si>
+  <si>
+    <t>Gawolri</t>
+  </si>
+  <si>
+    <t>Nosanri</t>
+  </si>
+  <si>
+    <t>Hwadaeri</t>
+  </si>
+  <si>
+    <t>Sageunri</t>
+  </si>
+  <si>
+    <t>Geumpari</t>
+  </si>
+  <si>
+    <t>Ssangjungri</t>
+  </si>
+  <si>
+    <t>Hopyeongdong</t>
+  </si>
+  <si>
+    <t>Jeungsanri</t>
+  </si>
+  <si>
+    <t>Jungjangri</t>
+  </si>
+  <si>
+    <t>Galdamri</t>
+  </si>
+  <si>
+    <t>44,010±2,400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -458,12 +404,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -496,7 +436,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,23 +775,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -877,7 +816,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -903,623 +842,512 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>300</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="5">
         <v>157.5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
+      <c r="A6" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1">
         <v>39.6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
+      <c r="A7" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1">
         <v>84.7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>40</v>
+      <c r="A8" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1">
         <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
+      <c r="A9" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
         <v>97.6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1">
+        <v>129.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="1">
-        <v>212</v>
-      </c>
-      <c r="E10" s="6" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="D12" s="1">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="1">
-        <v>129.5</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D13" s="1">
+        <v>128.5</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D14" s="1">
+        <v>31</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="1">
-        <v>130</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="1">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="1">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>72</v>
+      <c r="A15" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1">
-        <v>128.5</v>
+        <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>77</v>
+      <c r="A16" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1">
-        <v>61.1</v>
+        <v>14.5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>82</v>
+      <c r="A17" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1">
-        <v>31</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>147.5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>88</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1">
-        <v>12.5</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>91</v>
+        <v>54.5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="1">
+        <v>207.5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1">
+        <v>187</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="1">
+        <v>10</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6">
+        <v>33</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
+      <c r="G21" s="1">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="1">
-        <v>20</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="1" t="s">
+      <c r="D22" s="1">
+        <v>35</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="G22" s="1">
+        <v>40</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="1">
-        <v>147.5</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="1">
-        <v>3</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="1">
-        <v>54.5</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>114</v>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="D23" s="1">
-        <v>84.8</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="1">
-        <v>207.5</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="1">
-        <v>187</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" s="1">
-        <v>10</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D26" s="6">
-        <v>33</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="1">
-        <v>5</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="1">
-        <v>35</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="1">
-        <v>40</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all plots with added data
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/korean-archaeologica-sites.xlsx
+++ b/analysis/data/raw_data/korean-archaeologica-sites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CD044A-9CA0-AB4C-BF26-97C89F7DB473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EBF294-014C-4F4A-BEE0-15E676CDEF3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21880" yWindow="2500" windowWidth="21240" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="2660" windowWidth="21240" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>site_name</t>
   </si>
@@ -374,6 +374,15 @@
   </si>
   <si>
     <t>44,010±2,400</t>
+  </si>
+  <si>
+    <t>Hajinri</t>
+  </si>
+  <si>
+    <t>42,000±340</t>
+  </si>
+  <si>
+    <t>한국선사문화연구원 2018</t>
   </si>
 </sst>
 </file>
@@ -775,13 +784,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1343,11 +1352,34 @@
       <c r="A23" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D23" s="1">
         <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="1">
+        <v>127.8</v>
+      </c>
+      <c r="G24" s="1">
+        <v>86</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>